<commit_message>
Ajout du circuit de montage
</commit_message>
<xml_diff>
--- a/docs/Arduino nano pinout.xlsx
+++ b/docs/Arduino nano pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lolof.DESKTOP-J21SAV6\Github\MonRobot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F243F127-9483-4772-959D-EFA0A02CBE4E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5B57BA-CAB9-4185-80CE-3B50C036F645}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -872,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>

</xml_diff>